<commit_message>
se agregan dos logos restantes y se  quitan lkos datos undefined
</commit_message>
<xml_diff>
--- a/data/MAPA.xlsx
+++ b/data/MAPA.xlsx
@@ -499,7 +499,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3083" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3085" uniqueCount="847">
   <si>
     <t>UNIVERSIDAD</t>
   </si>
@@ -2759,6 +2759,9 @@
     <t>http://www.uis.edu.co/webUIS/es/academia/facultades/salud/escuelas/medicina/programasAcademicos/anestesiologiaReanimacion/index.html</t>
   </si>
   <si>
+    <t>https://unicarrera.com/wp-content/uploads/2015/02/Universidad_Industrial_de_Santander_Logo.jpg</t>
+  </si>
+  <si>
     <t>http://www.uis.edu.co/webUIS/es/academia/facultades/salud/escuelas/medicina/programasAcademicos/especializacionCirugiaGeneral/index.jsp?variable=263</t>
   </si>
   <si>
@@ -2922,6 +2925,9 @@
   </si>
   <si>
     <t>http://www.unicauca.edu.co/posgrados/programas/especializacion-en-anatomia-patologica</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAL0AAAELCAMAAAC77XfeAAAAwFBMVEX///8AAAD8/Pzv7+5OTEjn5eSempofHBj//v+Qjo7///0LAADq6ur4+Pg4NTLz8/MyLyzU1NSzsrHNzMqko6ENAADg4ODQ0NDY2NaYl5VAPjxgXVy7urjAwL7Hx8dtbGooIx95eHatq6pJRkWFg4FXVFGSkI9zcW9bWVd4dXKBgH5nZGMrKCVEQkAfGhWGg4QnICAZExISCQBUVFAsIiMkIx8wLysxLS6urqkYDQkZFRVTUVJkYFwREQ06OTpISEQSvlRwAAAgAElEQVR4nO19C3uiyPJ3FQgZkItAB7kjFwFBc9szJ5Mxm/3+3+qtBjWamERnsrvn/z6p55kxIpcf3dXVdetqgC/6oi/6oi/6oi/6oi/6ov9TJPzbAH6LQvZvI/g1+qbTf44favSh/9tgziYPFyaMQGtA6vD/HHx7OR0tFIB5WU9R+7fRnErbZo5HIPhuBFFsCjv05r+F6m1y8zLzmZ24rmv9aMr+mAkqgq9CJoAbuUsQhpfqUttzXS+xWZUp9r/TI6a49yU2cLYOw/l8PhrNaz8jZhGqm4e70SyCEhpdUOA6CC6vJjZH71cpP2/edOH8Cht370bSPyRdbbxWt1ywwHxoVm14+DIB/abSQbBaVMSk0RPo0HdVELtrAPmxP0kfWl1kmPNPfiexRu+fQZ+X5VKPsAc/V0FgFe+MVAKYGgUA60jiOB6ItzJ0JtQ0ACyHWnlJJ8waAp5w7nIV6gzzjvdIfOk6mKfWP4PevssWuO4I0HRMDfl9nqPnE3ziGYMgZK0tON3oamFidA3VkxlOAsUTk1FMl4Z0fQ2676DN39REenH/+gK7EqV/Br3X+KyLI+r1dURgidPjtTSF3KHXqahpMfftRQRx4Sw9Ez3Dg8rPfcaBLqjp8ynY+hVhTekOjPohddtqERkA6t+P3YwXaK8eLS8DcQzmNbUgCRjJg3JOI2BO3+JgNKrpk2U31908pJcyw3WxJr5W6Wfzxoapy/mOBohqXgBc6XJd+Fgmfyd6s0v4h1jPHGWJthdCnMKskDkOmk3ZGP0IiuFUeg+hmVSOJMXKbbY5ooJbQ1UiRiD1o4bkDwQaoJrhikXIOHohSv+Wl3AfJqhw5rSfTGCB7APLF1M779G3s4XAHpgX7oRgxqSy+WPeVGK5U9ViJZLRkUbGokeveFVcOsRBMwemyK/0Wgz+Hr0iQUhCDEhCWtg6M3RAyR+hoLFI8iXhYi9H9p/d2MsS56lCrOYSy3e3CCuc0qeWCCoxElNgzWy6rInntyKI8g3Wlo7isaf/LmnIOTgvcCFBJKc/Vnr5GOu4oB9uOWbNBC27fz6f1YaEKC5re3fIXCoCiBydhQhq8R2qLPcKdi0n4IXY2DRpMOxnjm/fPhG6qqrQDkLNtI1OA21kGuHEjNsw9jIZdbHD5MU1bC0trwBfynE2ywQNk1vRZ0vJCToDJgJYq3Xco3aQ9Q/7HNKtvGxWRjCaTIxLlIcZ1jGuYe7x9suTuNUyEpsKlFuYotafJWAel6GWrfqDprZV0WxbqEIbZmphVlPeO/G12GyUBu0aH4KJMQqM4lGx3d9THgR7jTjPcidRJjhZFX/99y5kHh9V+eyxAR812XNTSHX9KYWlC/6otr0GEQvmuuEDlElui3jter5BB2uPhfMIkg5WqQkBFAJzaNaCZTdx+PtZ/mhsFMVqiYHvTFn6F2L3sj/PIB+XMm8Te0W6IbWD6th2FOXZqvMd9xFjuK9kV8wgEH3PEEloRPcuu8J4KqerpVGaYKjiCKTsflnUufUDJ7ZH2oyDwp96rY6gEaI4DYnRFSmumqLM7ci2eQdSf3drwi1MFbyLfg27NFvyJgE7yPseVFtsDOzahSNG/hL/+/BgkvDxNOIrvTBLi6SJi8Swccg2ui8pCtBslC+p6uhuEolD0ityTxH/7FZCVKLo4sOSxL1jRlk7wtFq0NzAlI3+6RE2vyJBXWzpP1cKNtJamNSqM94JRKm6whXUmEgByUwpMOGJJtJZxX8TpV7oCUis7hr96Zrbs33aANzUIK15qxg6w0q/xSXbyUgbNXFeD3+rZWh61A7h8heMmuDGdEqJGfzOJt1k7UN+T82gRbKf9+I9LiYySQiYrteSVGhqFuTEBdquqdZ9K7bX2++6W6MtT3ywQtUp+Lx2jfldyFlbi5nPYpNL0gRS0pz6VvKWsXftSZiej15L79CtQ5VsPSGkyTWEbKKC9weiYVwgTipiCZLRhZtOnBwdlXQu3clztjOZukGZB6PaHHDzPLctFXxqB4zju2v3CmuC6bQ3iOPlDDHViLd8mHggldzINCd+jLP2V1jHC6SC3vpaE2cLEFG/vtFFGzuLD1/TtbO7i8oFKURS52mez2kiZXtKrhiMNkLbvEj3JJ9VZRK0PQeuMRNhmpGEUhKRTjGTAh1Rw1y6AhJLEDNSubOk+JW5V16JK9K5qrW4lKfQMB2l2MV87wyrxHHpRH81vRZJmvu0Xiux27e9v9fd5gr76dZ182xOmpL4xPW2qGicmKDX0R5bK2h5MUJKvcMKlS4T7jr34nyxQ6JsTQKCZlCUGNAd7Uy3Jy9dY161IkGOBjPBCnYagVRxPXKPGN7kW4y6v5JAk3/y625K58UNM2LAYGqiZEbROseSOClTl8qZ4P8gNie9Zr0chQyYSmBKW6ubY6d6eTZBHMlOQ8qbl7CaRoX/YpY0qZGD0nY8u8PMqQJ64Vp2jsmSpWJWOfgGKND4V1ctvTmDyfWRM9+mckWCNoWyc4ILcKKG2MJPy6s3h4/p5fXk5uqSt+dcedmgnPS4LK7o54eLmZH98N68k4T5KoJvk1bW3KCQljYE6AkHHPsRWaibd+i4fC4pocKCHiZdhXz4+BfHaLa8N4xbzgw4MybLm9dnfF/2ooroyqAzvh+9DZ/YXZr8aNDfUHfTX4Qkx4AmnzOsXoMYBW+BRI5G/SbLvfSg/0hrVRRN+ptIW+45RXQlgscLAYxWR8JwfbrMt5aEep55NOb1W58fEXcmkyKf3gjn0mSHfuCsOck8/86cz5Gst5MnXIXedVUmNbMEteHiPMFs95v/qYAP6Bn9nNuJApItwydhdpnD48lic+0Cxmsti7nLBiVBvpCN7W8cvTD6fOKNNNkZMsiI7WXO7LFXT2v5HvLyVPSGtb4SVl4eW6Rv2EgSV+zNNSfboMdK/mS6Xg7ohQVvfw9Vc423DlnMkae4hoktOyqtj5Aw/nNSuV3uWDGQuaaTqOHKO5RzYr4B/ae7st2LAb2HBQlHm1QFoDk7dkDWcm8ihAEWp97KhJmby/7UrEBaDDdHDUofqCsH9J9u9m/RO3Oo+dTeN4+5EqAmSzJ17PAM379LqoZdJhAKsAr58L8eQUVdR8bH34xeogFm2DDmWod7k6lCA3nuM/0cJ4+cwSipbKhdywnq0s6QjUjgegWcjF4QwCezBaZkepxgXG/Rw4wU8iItUbHTbCIljg9lRHC42+hUWkdgOFEGSZmTrSCxrFb4YBpNT0OvxyJ0f6pR3140ya8eBRDej5Ts0Odk0UGi1Fkudb7phBKsLLmGqj0ZPJ8aVpGGZMW5PqwK23G5PyPjol6pPkCvaqltRaAFI4lbTVKtmHMbvEmUvX3NHnoIZW5aekl+k4JijcBEwad2nJyM3rriQRoYRWB3NOwrkQxV3Vn1s+wH6LVUhEixNBC9+5T3dmyvrfVUIH11JMHb7f+MHuq5pWuS7sqQe08WEPQuF8TTxRx71KW86B0ARVSJ4Gv2/KYZ9KR30U8Fl3QS84bJoFoi8tdlEnr3ejQDLrDm8ltDYA89xLNJk3jUX7acgjTWAd2p2vs/T6JM0R2Te14CwUSrEiA3s42h/x56LceGFFKSU55pQ6lPiVf0lTZRZ1DJkNxRc0hvMcA+enpRmbhOzKML0G5ciCZgQ3FyzsDK1m3I7lySnK6LSSKQsH1yP0I/HQFb1U5K1kzndB7bKnZioniWwuNxo4rNQT+qsHj76EkrIMnj2igm1BYOxsCgPlXJ1IlJq1gka+hPpTcXemzt++h1BokkxReFSJak/IrBncqBeBX6Kml87EiM5wD9ff/z9QXJ2vqngSOIS/BPnWvp+RDmYG/ON42MG/x376IXWlKnbYjEC7fdj8LuaezaPE5d3jTqH+7Lyw/Qi9xvK4bz4RX1iabHa7AvT/Qrk0kF6DCItn3coq+bm9nuOHoC6d6mNNDm3uG4PDBIzUkCiwV4mvHKdhzQDyPTDUCkR25+8V1QCH186mzr0Im4kD2wtyNFW2Cz0ZEV5Qj6mHv2yIyX3Jcsc33wMrol39GBep2/hG/toRcwRXmLtSQYUVEQw51oG0Yo6H7o5y6kOzFlb0PZR9s+aWhUJBC9lmrViwh4QlK0ulBz88XxffQEYMdauQ/TqC5bsjNOjKX/QDWyoRkRI9S7g9s2PNr2JKZaGphH7iW/MiSlnF+d4CHvW7M99HuK0X91Nb+/hpJk34kCn2HMfa85LsNuc0jceZreQC8YpX9sWDHj5RG14QrEnx4cwD9ED2yL/7bGO5qyoyZ/FVh6g3Ic94aMHnHHZM+Aq10nvEKvP/Y87B2Xx+yIcKUjSgdxuD8kXqC/7J9HJ3gs4ad9wwc8UcvMUa/1XUMu11Niiu9voq8k0mPfzP5rFfvIUQ9jmszcvc46RO+1aw1s47lBYuad2vY2jdpndr2LusyXqq34eYV+naxxdtzR4PGMl8WRHxaMdC5tshdNPETfOXFeZOwZfU1i/ET0EUlMf6fSKYxEqKTeCkfRC7q7etTgqPbrxtTI7uz4Q8QFJnvvPKDfyFH3HqLvEqQ7XnFIgLyKnL5BDoHTRzt8JB3cBJINQKU8QC/zab9SjrWLRmeuWzJUjzCVkGHN4r0unO6jLzQgZTTZQdCWHNSJ8l7i0sxebmWCM7x1Yx1D769o3jSPuV0dg7vj9cqHY5wfiYs0dJ4zNffR532bP0+uMReW0akKvknDWxfy2yIdXrfgIX4Qm2PoSXIHo2P+aR6ITYhXgykc1W3tB37PHccN6IcklLD/feM2nnbGLNYFkO9OjZ8vGQhVbl/1ek5iFFmkuRLI0Wv0/Sc7IsvM2wvdRYVagmufRyhhXPRs55N99KlGmpBn109hP7v6RsTZMx0du8sxalKwRC3r4zVyEeW2BBLzYPUK/RSf1E187wX5NLrTG9KHV2AfnyR16pp4Zys+o7dKiCOXDCs770W8goruSRCcbJbLZI/fUfsvalJoSxZLnAMzM6peolfAbgI8xvUjqwL+Q6u8aZHmaHlJoL9EPxI8/hzdteXmnrRlknHXBeE42Qs7pfEdIYYhMW1i+yFeEQ/qKfCwr9I+o5/eY1taR2XBTCy9v+jzJgkMMI8JO8FPPA3UDXpni95RoOE/IqY+aX35VbpGkiLJ6dnAOh8xgW/uJELy3xsRbCcqD9HrIPp/Lo+JFEBRqXi/T+q8IbP++HM8tR3ZL9CvTVJLXVzvXljUU3pke3/8FscoJLPKutw/UqIuZL0ncA99L1NfW4E8MWUsRgiCBCMDaPDNj1oWjUNS0TYP0EtrCLfG6BY+Z727M8KGEe+n+kBWXKdQQhjtoxfrmAz+I1zRCjDTtAYSF2joZOwNP54MraGtD9HLdpLDYXfWOQ+kvTYm3ySBW87moXr4IDnWj3YffZwImSMckQXRUp1IUEGqExpIahJ/x56SNxibB3wfw8htJSfcP8vhoi59pWi/Ry03dZK7/UOsEiOv2EdfTnDk20fYXmzm8ynpaCS6nAiE/6QwPso64vPRHr0R0yUppPtWlMnZwDwr4km8xkExY09FkUaQSzNQsh16uq3F7o+IHLFUuEbI9SWT7tNMSan84IHJDn0GswMgDnwDH8/L8WpvuNNF3lNL9RnE0nIffcynoWOJ5wrr46vVE6kQYg7cNsI3n2QeoldlYc9zE/WTiYlnLr4R+9Q8SG6DXDL73H/zDtzp4z56nx8+whIud0FTx8yFGxprecRPCo4JTSWXrxfdAfqlKIk9ekEwXX/2h8YdV9nDeeC5STewRFKOVkbAMU3ITPP30At/Xs6M1RHNPgvBkwjzY28urgowfWqNIy6B+aJqc+UAfRqLJg9amTfFaq4M1zinGiZ7VDxRmw2+pY5HG/NK1w13D73JNC+JjwQigwhq2wWdJvxOsB5T0SYNy+5en5hDnpmVuo8+Iul0xZlp1AtZk+YO/eGoxHqfJFIABSnJZT/nOUtQeFKvsu/Q69Ub1k4gQVslINLzmV6ZkpJyoWe8HiApU8GyD9Cr6IoVjXRv/n2qsNwi1ivufyW31MEavrG2/qvwFaOoCYHBIz+LfQ15ekx/LEVIIksS6KQpEAd1wBvvSGrf3pEtepA7EMfXN0WlGE1d0usUF78WXo1xZA4ywZU0mux6K/kZvW575YNyRBpIBCIWJNdWsrruZMcDHsw5MquNIlffLFiJt+jVm4TGnD4VoV8oJP3n5lfjk84t+qaW2z5z6J451+X30Es20KxwTJYkgpmnLXM009TJzihr4o6X+UacsqoxVnM4QA/aVQxKkMiybetiifNfD2wLCl6GjHTkUouNTuDS6xm92GYoVUedUErTp0SrphQRlNzkIYnXpPIJVC1foAdzNbc86jNbnuN5c+wrytDvEOfFQzcdYgZKveN7j2lHl4qIBZdwcVtXTPbLurJ0leXHTKPWUKJF8hI9d0n/XBeIdXnuLPWSzEkI+lIWdyj30BNp0yPweQpi3sUqSL4qtrpXhY5rHMnx0FS7Czdq0gF64B07Bz04NbPibarRr4tnHX4f/fQBjdkrsclsMBsyhevYsa0md1gJRSOWr233qHoeCwP6Z+vPW1YlHnNKn0vTm3TPDbeHXpw41PKvOncxhUKSaj8q/ZCFJbFPVrLL8sfLxv/2Dbrdq79An9+KxupzFr/ZOPtxUW89gc/oHYs7zF5pyPm8dFq7LEfjoFYqJStwpIzi21dqphay2g+9I+jNpixnp3r+PiIVpVUn/9ReoodsdYNHNIU1snphjDoGrpOpLM5n80d/8sq1EKdZpuTRa/Qe5uGjtPwc8OA9SWG88De+tHRv1HrWMZkjdGPDKLtRxJSqSphRLR6K6JWmpR7MQtEzen1elslIP1Olf5Ps+1BSwmRwLx6gFztDA+v1YxIDy6rOTXDNaVeG4Wr+WsX0aP6AHXfsofc9v/bd9PaTOCcbqXkjjYr2FXqlchX5qJ/Iy5D5jYNRSW+Cr/KXgVuaWAnx1lWwRU82RdOk0jo2bz+pHMBoPkOQVHuevkQ/tZuxIh339LURixZ+bbdt84bvWvfHi20D79peDwtHFEUMitMzct4l4u30CfEpaZ0X6GFiv8mdLFKS1J7bcvZ2Bqe+U/p36POc8Rxr5VMrSXS59Oec9+Uh+ne8LDGr2WiEy+jtihDSczz4ue394Mksz01Z/4BKGaaDD/kA/TvkjhEffyTXNcama33kTNrxPQg3ZNz8nnL2itg1DCkySncCehXMeKVMQb81K7cb493qvnkf/7PMych4a35jkdgxSlJwY27an4QeottevHr3WlqCEQimlwTv8vEOvYiWCMsz/H6nkBXA1OHOxJPQa4PjzmPulMnDmtv4+qiveUs79NH3xITPzvf0DNByfveT0GeK4uimaTfNPO9G9V1d5KrxbvL4Dn3JDZnPRj8tQOxvfAp6BxMPTFGUBCUDdstYlYd29+5IHNBT93SM5M3vFB7JWfwKnd+CplT+SejN53QOZqn2o2wCW6Tv5xns2r6wSe+7eXWuFMknhn5sXGFzqBGKqJku88uT0NtbW9cUIr9iC5eBMkHl3ba3t+iNqBKF6Pvhr+49Pp2qMQuYaBXqoLOs4Y4+UWnJgpJjr6pPQp9ndsGTS0i5p29l0HppU2XRu223Q39r2yKD/OaaZ0qI6zCLuMocqf78NPB8yZbmLdocmRj3gQDnlrm1wyCbn9b2tWdZidyW9TJtSycvw65G9/pdU2mHnh5q2bLXNiJfpDNzpWrpXLFYX54cM3QQIhcLUnCtoD+gxrOaTMAAT0LvD7FzTdIhyqWim4re1dpU3h2JNjdGaNSKWEMMQTGMHB1NF6QLVG3z9ExeEcVED4HpcbXeHDJUz9J8EvgnoC+Ys0Gqh4qauaNOMabW+zl9W/RRmQpT0DbLQ+Emt01bXUN0Rha1OrZsEHJJcbaRZNIubai0LjoF/bzqeiv4myu2cZiDGvIVU+N3G2+L/jqKI8Hlfome/JuIJY4IyTY59BS6SkQwZfZjtvFJ5CmpLlLGEwJPGrXD0uYuIskrMR7xK1UI3h8rG/SdAw1/89VGVyjWvsWzEOWTBy0NfBoizBSbrcnNK65IYwtYdgp6qVdG7eKWjCrSrHNXwkKA0Tuc820zam2+QCEPqJd2cQHD162Y+xbPQ69AuCuNNEmc7Ka0uSQ/Ab2+cwcIdlIGmdSOJDDD9y7ZoV9OoVJulWm+0SvsJTEdCd7y/ctfovcceZnbq0FV9THIeWYs66B6/BC9cLP7s9ZIViGi9JHSm2/QP1iwcIVquYku+2Ek45TpvVlxKv0nAt/tuLdjNUgPzoqEvs2gCj/Wc5aSuVGHY15qpkgl+2H97hWQb/h+EkHtwNYsdLjlKHZezDWVk2kVQav3fBptUvq+UTv8gLVyEnov6OKKD5Xcdxk1Jrj5R1llW/RdBe2zkjOMXdGszlremNrA3zUPW/s5N+MxgTE7CT0kq6njNjWL7UD2fZL0i48cqlv0181e8q+Ocd3xd2nPshUrWeUBv8SMx/2telF9J+qkKZ2E3uW5KknG1wrTv0YmtfUk9Dnkt9RzsCmSqC6Wls5d5wtIj6UwvUFRK8rgD69LumHOO8AOSVui4XMK+kfBccEr0zbogtpyXWg/0lK26C269XePN7sH7TBlpTGhn5+h8UsFoTcGVg2eXERH4Pnv7AlOQp9XPEsInEZuR37/2A+TKbfogWwDCz2V4cSbDDI+4jHH0xUF/jTdh0k/ZOxMwpwUJRLZsKL+r+Yfoo84Vh5hDpN6SdOtpSYXHz3wx4bvoVZ4KicGZovCz14ttRsSvI8fXH9AWVQC16xBfXDhaTpIML6iA1jAXeLv9WM7rhmIdtOSjLflSNAz0jw+eiC/LcwinhPHH0X/8gXYvZilu5XsXZP+JU1DWfd4c+QhT34fDj5y6Wvf0n8Pb+vqphG4tQfTSrPtQInkG6k0w4/FXUnPUK+4fDE2A5xnaDw4fWKXFS/PKyVy7+R8bgJStBOYp0kmQNwzL18BBes3m8LD0vdaHq2ToQ2XVR3kkXFCwz3ylWW98ZdQD0+vk1EGU65XAc3y/vtrFF9TXDgehBnPh3N9VaH7isMqHIlzTfuWnzFG2/b5AicIcxYtafYxvJPCltxHrg0M2ZGSV2GuXpsgLfSghNj781wPybwVNZAn99R3bpZJIM4GHVXnQZC3tG2GllRaIqnTqiwpUyPt0pLXrfmQRN7syRAuEZY0RJ2UwENe3NggiaOzg4f6RcqTFPKu4kV5SIqNNqoLzxNyj9tplaH6Q+KIxjNVPLcLmVud4pNMeO4U27SJ+LMvOiOSncUd7FLxgY50jMTleDfFuCnuljCUXHufHWPlNgWpHIZXzEaCJvFOyE6qJHDNBUO3zSXXC6x2JV9kPEM53qMSMWVOkitL3Fuc1q9Yr1avT88qsNb9BA9aSdZFToJWuzhJuxL6JL69wFx0i2vfdmJ/jb8c7RdZQ/bRQ+HvC0idP0l7nTpd8uSazXWKLCY8oqbjaXI65xw/PbDbLeXpAfGms3+r5uFrv3XNM+Gzl+FUQedtPvzpLzZrr/ITOXbM2/fkNai/RR63e0x8myUiZVPpVr06zQ9f8SU55i/kzv0KFXzOjd5aOSfkCtv0dn5aa1o97jb4FHAf0rQHnh1zi6okY/OtIXGi/8vtswWk0xeO/yalPdPXR8PMPtsNs9VJQ9Ydqnutfk0u/gLpd/0DZWxfjmn39tkoPZ709ZLsoTRP9Q/WafeGxJ/pBeYH+IX1c/dPT/ECuM2QeZZ/Gt+cEqN2BvhkAqG/X6BurwE/bkvV6bCv7k8i4GMmO7FvkmbnA36bppvCj0Je4ERJzo8zuVE2xnrjc/oQvBQVpwZBF1gHl6MyetcWFY1tIMqMapoVja6sZPZMebx7nOR5nmVNkySO7DxncqV0E8RxFg/Naa6PrnnakcfSyeK0QdQT6fWgxcrTZfYeNzJc7X7+5sbyddusJldjfKa+VHiz+3q1DEbzMF2015VtbYWpWuHobe1dZCtseF2J1Rka/mZFtpDMr37AmwVyTQVn7C2e0QWQZPRlVCxRf3MomTLevu0s0eubvGcA4f6sQd0aJo1eW566xXvp43oeoFE54lu1i6Xby3fYT4w6fM9q5MUZPb6OWPp+phLhjyU3hk7qvVHvkWanF3g7avPYcTVRNIn057a29h/7TdB1U9Q4eTHrlrhU3huK+tglE82H2L46s7i8F6xjs6juzSmYpMq7df6eHBWdvA1Xs2eGH9/d3oz8DTSXhctboofLvSFxNS9fh7SfyaUZu8pJSk4XZW4pf7BTxPiG1EXg8oUP8JSOQAw96GI7OFpw4JB0TeLCxUmSyLblNXLbUu+w8Xkh4jhOksSZWpbnutoHYJjhM7i1Ie5GtUQC6Vu0OtmPKd5vtN/YgBb0OQNeVDm6PZaE/h5pTyiJ+MfZGRN6V4NXiqS8RbbTz9iC5p1o54B5h/e3Dz+D0Pcsjy+eWpGNyPlXvn2z9NAbFC6N89eMsO8xqCNfomcKUEVJOZqNuqx9PG26iiJezlgVLbZ6snnoD8nGDniam5sv5bOUKf3nWSvsgIvQJ1mFJGhsaeZwVWSZJr+a7iLVgQa8QnSqZYGpMiba6/IcAZCf5X/U424u5ypkqWPE4TIGd1n9+tIHIufSWzEHSXRer8y80nme6OPJ0lfVT+8qM+qIXSCNuKdOG81+3Grx8nf34XDRIMnlYxnjNBo0Gz0PO+9zN8gQWVj2Xi9wfrhX1ER/eoDx999PyYwHDdzJr30P/LCkweP5dvhBTRKuQHj0goKn86J7H1D0PZpupgc3jidKWPMFwZ+yNdNGVpnzCqIHEvyNI1gW3L53CZvXNGamE8/NIkx0Pj299wYCmmIZmaYcINPEKBg0n9tPSSmdD+jtkT/4Z7xy1XTF+5bcXcb954vYvgOjExXTetchZuIicezOYALfByUaTXseuljNYYYAAAzHSURBVP2UtMZ0QO9NbFXEdFizoeWX715zlZG9NA4EM3bRMzUYvTtKdKyUMudgU5R4uLRH//NTRlY7zLzeKI6EsTyqubKqy++XliD0fpnftqAVkvXsHX6DVOyGJVBB/eBF7izqv80+ATs9egDqTaJKXF2TxLxUPF7u4j0izlk6EKXq95yRsoHvxz54oW5Qo2CSOBeRrBnTfj3vGTkt75A4ZDzYy4Alg5M6asYX73qa/DpzpqFSgp2mnQ1C8UG4Fn3WXHB1Ob6LtGnTF1uyP2O9EhG753fz5iz6Y6zoMncoC0mLyyz6hJRVQYra1VW4qSrIsA1u5r3LevZZ+bAtD91OO5Ibjz7IT2be22muXV9cNP5QZeRXyPTsam6MqrifUe2sL8Bh63Jvs9SftHADuLOosXPutwxbID5OWJYMxWdEh6XBwzKsbO+Fzn6w080Ly9GUElY2xTqVB1eKl3cOtCiCwFfP562rx0+fuX5AZw3fiYt7G1gGiZujUNX5dGh1QUvy9jG4mq1qhUWO50qm/lLaqaopeU7Mqmxu/NWkle1sli4KeZLUEEdQ8tgau+Vehma1+Fs2eatbXuk08aK2trx4lhTMfJ7OBc2KbbnMumLZG3+ToKfJbIx4d190dVvZibcb7aRAJMSNrcAXZGvgt7cqxE9/5w5jrBPjObW9raLtJSMobCGQOz93pVd+E13UJNd1JW6qv7yNxmKtr6FIFggTetPHLT2aHs5JgTqfeBEeloZgg41u8hePL/yA/2hTpbrIM11SbMlxXfOoWqZL00RifWRLW+u1B4ugRx+ZdE89ryT9OtbDM9JwfoG8B2oxwSQBPnaTgjQUzyJFKPK8CQRyDZHs4jRdyzQt2BEk4fX1lO+KotAob1Lnrl9XD7DIQUtU+7sHQQJTqWx02cr6FcW/v6D2fTLrSy7RTIhchioENOd2Cx80jJ68eW0lgN+oQ8IIVguesvKNq7mrmKfMsCSCdd+2vG4heMoog4aBbKpV2Q8eMQv//l31pBJnCo/6mGSt8JUKHY1i7coLwftJ2jQKLCWpZ/J4As2zfI8kQj9P5IYU1PWUZ4nx+jjTSHNQYxhu40detoze9jp+JjnlA3a9UqhLYN2U8cq8BPRKmBqE3k5p6nHtux8cPd+/s4jpDX0/t3RCT6/b0qxh3WvTyoIh9dFMlPFH9s6nkmZ3iI3vDMrh1M6spklztSUesQwoc2KsgKPnWjqhv9H9ChqzYPFVv3uSs7V4BS+v77D8Z6KdB+Tm9Qxx1NqbMjS6FuuxnPidL7v3boJeQX/xDMEFWU6tIleWPbV26osuxSydoNHan7y66gzSvfx6dIWXRSrbU+1Q5RGkDdQDbtZFL87b9Qxvmir6za3bPodMl5SFJvgTH4wizBQ5j5KpRSpDT67rWdMkypms1PNgdrUs0upHIv3vbSSsa54TMb9Nw5GxvLrr/cl/zibBX/MwzUo/j6a7FOUv+qIv+qIv+qIv+qIv+qL//0j8ZatIOHD1mVa0OJKXvSHNYfPTl7opo1HTzEfNJok4m6y6+dHLNTy9QvQLejoISEQBjt+sXipck51w+tINQTRvLu9cYWvmmSXGR73cLuKv7s14h4cJ1ja+XXsVoMOzPITp5X6CgTl+47TkrED+Prns0DDU3kXPzkNfj/ejasLyb7fm3kdvHyts9jYdolcnf3ua7fvo899BD8Hfbv9r+BZ3cmJ4ViglHR9EWN9E756QxPEqjtKTcOjr1vC98DU7r+Bhd4h+tEVPgktNKn/rctTuEhCOgBPiPN8J9InGt/zgZ6lx5UdDrOVb0x5EszTclu0WpvGrCnhnom8uDyaPZhPeyUb9GnfER35/Tb7DBOzgbrLEwIdpMzEuJrz4i41KZI9WwytfowSPyBnXQ8XJkUdKTHtCBwb0UUfzCXO3nMOwG+FkG04y5ZExyhL7PM4JD9Gn/d3cDosic0HIh2VETtdDgRg3dSrMuz4ZRhlSU9ZX9IpJgSjOeVYvmL3Y03/SpVI7Hg/o3WVAnSSFeDWM2gXf9pjhH8Nzc+Qr3pLb8eVZo7a7PFgFwrNKwSzw6mrIqPU3m2Wkw0oXYzPlCv2aiGSTFB2jD2YWPPA9x1xbh2hI9El6IPbQ9h5u4vntMNcO22iZeCUMjxnmE30yPgt9Oj5Av6kK8WO7hbq32Y91yBUkXMPXYcHAHOM4yv3rAGf8693dZk3G9ixx+NKjD7ZV+d1eYhLs/hv2u3O7uBV8/plz7fggma8b+NDZ7k+iYbCPHsZDCcaM/y/hOo556qgz7cMixjY/3cRLI9pOewN6C7cMKiISn1nf7Q16fl67W+bGztBzgMv7A/TpFv1mgbT0An3V312YD7gOt55Z7TY9SIj9v7N99BXuijSNn7OnTDag/75bgWXjWWmd9eVyX2ptSipPtwsW3Q36dnN/sR+3Ud9wDA/3hCqeVzaJyhjRMAf0CqGvd3Mood/M5+IitAbOwd2VMZ61Di67vNhXbTarUz1sDtFn29ZJeScPazlyPFz2VRysYbN/DswSkQT/Rpfttf2A3uZLKnr033B3ZXQeeh/3i/WYG9BH0G+y+i1cgjuMLOKPA8tjh37IJTFv+gXeA3oft5UGtpzDsC+m0Lf9bLcaMMJje3y9SR7ulzdj+Qv00kZ87NBzjJvBIdw9bLOaerw79JvdEYft5SJC9o0/ZjukB4lp9QPVxL7nFdzqtvZ5oxYWeL9rfC/49gK9uZEVz6v1IjS2lTplxKH8cNS34GiLfoqbm4g79NCMl9o++qDvt2uc8ZKxJIfqX0NPL36R9/il6mnzHgLJAkunh2o2jhORbNMZbstJq8vnwZkiXtXMD3itJVWboSL12SzSIG/DflXh41BPTpzhn7kkSvbjn+jp3wS8S7Wkc/Ey43u0xIjrRBQ9f3W5PjNgZJEe8GAsed2fgVgYdt06tICtm65rGrtLs+u02fzM9hbc2vckG+/5D/F6ndZpl3KuEjJERV4TL0t0ZbtouGTV215tinXEcSeSCMVLX+XKVD+IvDXPlGldeo3lGSVoevrmTqfWa7vk+BKZw60tde2oTi05r50QqtZPvkMOJgjfeCYS7LKv9T6Iqnn/RAbAF33RF33RF33R/wC9nkH/r0yCCWuXT68PS8d3cXcj5jP7k/YP+ARKatLaXh7UJ3jEf6oy/MkSJypJx/3dBV+fRjYe2QiDvUafPOCP4S81w787vfVkmuKR/Sj1h5foSft/bvD0Hypu8jF5eGTJpnn5Aj0Ztntr2PX3/PL/KFl4pCHNF5yjX40PzLjPWG73KTTFI+LFfBHtux6fs+fmP0gOHqmk9IJzRLz9n+H0Z+JVBnYeX9BYu5A3m9gejtocx0c9pq6v2P0Fui70FQvoUxC2VqYWyX7ubGY+j079zFCTlBXFKGjtbduzcS658uCffoG+vju2fl0PA1Ziz1L2CHsvE+PFRAankRbiwl/hEHQw58X21M8hhnw5vNniw9bxrQ2H+yz8Q/TB7ZHqVeqS94e98WiXWx/ZppCKi2OO9Rr5e+tXSn/rI5s3/jL44Y92cEJ5m2CD1jPSC743bo8U8ml7N5+GP/tv/hZ9N3jSJpveivmS+xoH1/1nDR5xN0c5wz1TbJUy69Z3yJ/0QuaMbl9vkeAOb63jsKRY3rZG3XeejbfPqp41uKnNT0Mv79xww2wlEH/y1G5eNOTbK3mf3r3OvJh2vbNH3aCvtlGFtEcfjveUCWfYn17/NPThLoTh9b3g4UFE7gV6fzx+w+uVhHdDeVi23aWw69Evx6+clEkz/iz0k92WiG6vpU3xoECueRjllvDhaO0wx/BdHAqEV9sbzo+jTwwmfVrbB7s0lgG9hweL7U083Bu3uXux9Lb/Vn/XaAAN6Mst+qZHPzqMbAudIe4CY79P2W6OGtCLh0UfzRdqs4eHJQT7vTa6nwKXOQN6f3v9qJfq/mFrNBP4TJnzHAwZ0FPr3m4e5/b1Dl9UWmYHaAT+hfVySNqg30a+1Vl/Y+15dtb4u0xhJ6U+g0Z4Mejr1oDew4eLXlDbDyJHP3txvo13O/1eNGigqxd9WcfR3U8Q+m2UfhLHfMsLY5gaqPGHNIT2ml6Wv60WjA3QfzVr7JD0ALGMp3Y2f3hweGvFZA1ePD7y7W1Nh54dvdg4W+qQF5AHVZORt7OOl0XsL0g6zZfeAPe/PFGB7nvFh8AC8S9ZbnlozcTLJqkyOrWZfZKyoLLg9mbONBGDri+ho7XGbNnx9meVnDO/fLk0U5TXYRoat8Ei4lNn/hSEU15NaLPnij0PeCmYNt/0UTy/xdt5r2Gwp4Dvj2kby09cQDbU+t1bqP6xJ0Q4o4AL6F9Lgb7oi77oi77oi77oi77of4L+HwTyutXIgT7oAAAAAElFTkSuQmCC</t>
   </si>
   <si>
     <t>http://www.unicauca.edu.co/posgrados/programas/especializacion-en-anestesiologia</t>
@@ -15407,7 +15413,9 @@
       </c>
       <c r="G454" s="68"/>
       <c r="H454" s="69"/>
-      <c r="I454" s="21"/>
+      <c r="I454" s="37" t="s">
+        <v>752</v>
+      </c>
       <c r="J454" s="16"/>
       <c r="M454" s="8">
         <v>7.140247</v>
@@ -15430,7 +15438,7 @@
         <v>22</v>
       </c>
       <c r="E455" s="71" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="F455" s="62" t="s">
         <v>180</v>
@@ -15453,10 +15461,10 @@
         <v>749</v>
       </c>
       <c r="D456" s="33" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="E456" s="71" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="F456" s="62" t="s">
         <v>180</v>
@@ -15479,10 +15487,10 @@
         <v>749</v>
       </c>
       <c r="D457" s="33" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="E457" s="34" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="F457" s="62" t="s">
         <v>180</v>
@@ -15508,7 +15516,7 @@
         <v>142</v>
       </c>
       <c r="E458" s="34" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F458" s="62" t="s">
         <v>180</v>
@@ -15534,7 +15542,7 @@
         <v>62</v>
       </c>
       <c r="E459" s="34" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="F459" s="62" t="s">
         <v>180</v>
@@ -15560,7 +15568,7 @@
         <v>66</v>
       </c>
       <c r="E460" s="34" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="F460" s="62" t="s">
         <v>180</v>
@@ -15586,7 +15594,7 @@
         <v>166</v>
       </c>
       <c r="E461" s="34" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="F461" s="62" t="s">
         <v>180</v>
@@ -15609,10 +15617,10 @@
         <v>749</v>
       </c>
       <c r="D462" s="49" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="E462" s="50" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="F462" s="62" t="s">
         <v>180</v>
@@ -15626,7 +15634,7 @@
     </row>
     <row r="463" ht="14.25" customHeight="1">
       <c r="A463" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B463" s="74" t="s">
         <v>87</v>
@@ -15638,7 +15646,7 @@
         <v>88</v>
       </c>
       <c r="E463" s="29" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="F463" s="62" t="s">
         <v>180</v>
@@ -15646,7 +15654,7 @@
       <c r="G463" s="68"/>
       <c r="H463" s="69"/>
       <c r="I463" s="75" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="J463" s="16"/>
       <c r="M463" s="8">
@@ -15658,7 +15666,7 @@
     </row>
     <row r="464" ht="14.25" customHeight="1">
       <c r="A464" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B464" s="74" t="s">
         <v>87</v>
@@ -15670,7 +15678,7 @@
         <v>428</v>
       </c>
       <c r="E464" s="34" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F464" s="62" t="s">
         <v>180</v>
@@ -15684,7 +15692,7 @@
     </row>
     <row r="465" ht="14.25" customHeight="1">
       <c r="A465" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B465" s="74" t="s">
         <v>87</v>
@@ -15696,7 +15704,7 @@
         <v>142</v>
       </c>
       <c r="E465" s="34" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="F465" s="62" t="s">
         <v>180</v>
@@ -15710,7 +15718,7 @@
     </row>
     <row r="466" ht="14.25" customHeight="1">
       <c r="A466" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B466" s="74" t="s">
         <v>87</v>
@@ -15722,7 +15730,7 @@
         <v>62</v>
       </c>
       <c r="E466" s="34" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="F466" s="62" t="s">
         <v>180</v>
@@ -15736,7 +15744,7 @@
     </row>
     <row r="467" ht="14.25" customHeight="1">
       <c r="A467" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B467" s="74" t="s">
         <v>87</v>
@@ -15748,7 +15756,7 @@
         <v>78</v>
       </c>
       <c r="E467" s="34" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F467" s="62" t="s">
         <v>180</v>
@@ -15762,7 +15770,7 @@
     </row>
     <row r="468" ht="14.25" customHeight="1">
       <c r="A468" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B468" s="74" t="s">
         <v>87</v>
@@ -15774,7 +15782,7 @@
         <v>173</v>
       </c>
       <c r="E468" s="34" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="F468" s="62" t="s">
         <v>180</v>
@@ -15788,7 +15796,7 @@
     </row>
     <row r="469" ht="14.25" customHeight="1">
       <c r="A469" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B469" s="74" t="s">
         <v>87</v>
@@ -15800,7 +15808,7 @@
         <v>30</v>
       </c>
       <c r="E469" s="34" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="F469" s="62" t="s">
         <v>180</v>
@@ -15814,7 +15822,7 @@
     </row>
     <row r="470" ht="14.25" customHeight="1">
       <c r="A470" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B470" s="74" t="s">
         <v>87</v>
@@ -15823,10 +15831,10 @@
         <v>749</v>
       </c>
       <c r="D470" s="33" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="E470" s="34" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="F470" s="62" t="s">
         <v>180</v>
@@ -15840,7 +15848,7 @@
     </row>
     <row r="471" ht="14.25" customHeight="1">
       <c r="A471" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B471" s="74" t="s">
         <v>87</v>
@@ -15852,7 +15860,7 @@
         <v>191</v>
       </c>
       <c r="E471" s="34" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="F471" s="62" t="s">
         <v>180</v>
@@ -15866,7 +15874,7 @@
     </row>
     <row r="472" ht="14.25" customHeight="1">
       <c r="A472" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B472" s="74" t="s">
         <v>87</v>
@@ -15878,7 +15886,7 @@
         <v>66</v>
       </c>
       <c r="E472" s="34" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="F472" s="62" t="s">
         <v>180</v>
@@ -15892,7 +15900,7 @@
     </row>
     <row r="473" ht="14.25" customHeight="1">
       <c r="A473" s="70" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B473" s="74" t="s">
         <v>87</v>
@@ -15901,10 +15909,10 @@
         <v>749</v>
       </c>
       <c r="D473" s="49" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="E473" s="50" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="F473" s="62" t="s">
         <v>180</v>
@@ -15918,19 +15926,19 @@
     </row>
     <row r="474" ht="14.25" customHeight="1">
       <c r="A474" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B474" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C474" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D474" s="33" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="E474" s="35" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="F474" s="62" t="s">
         <v>180</v>
@@ -15938,7 +15946,7 @@
       <c r="G474" s="16"/>
       <c r="H474" s="58"/>
       <c r="I474" s="76" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="J474" s="16"/>
       <c r="M474" s="8">
@@ -15950,19 +15958,19 @@
     </row>
     <row r="475" ht="14.25" customHeight="1">
       <c r="A475" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B475" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C475" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D475" s="33" t="s">
         <v>22</v>
       </c>
       <c r="E475" s="35" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="F475" s="62" t="s">
         <v>180</v>
@@ -15976,19 +15984,19 @@
     </row>
     <row r="476" ht="14.25" customHeight="1">
       <c r="A476" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B476" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C476" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D476" s="33" t="s">
         <v>30</v>
       </c>
       <c r="E476" s="35" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="F476" s="62" t="s">
         <v>180</v>
@@ -16002,19 +16010,19 @@
     </row>
     <row r="477" ht="14.25" customHeight="1">
       <c r="A477" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B477" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C477" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D477" s="33" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="E477" s="35" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="F477" s="62" t="s">
         <v>180</v>
@@ -16028,19 +16036,19 @@
     </row>
     <row r="478" ht="14.25" customHeight="1">
       <c r="A478" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B478" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C478" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D478" s="33" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="E478" s="35" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F478" s="62" t="s">
         <v>180</v>
@@ -16054,19 +16062,19 @@
     </row>
     <row r="479" ht="14.25" customHeight="1">
       <c r="A479" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B479" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C479" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D479" s="33" t="s">
         <v>237</v>
       </c>
       <c r="E479" s="35" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="F479" s="62" t="s">
         <v>180</v>
@@ -16080,19 +16088,19 @@
     </row>
     <row r="480" ht="14.25" customHeight="1">
       <c r="A480" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B480" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C480" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D480" s="33" t="s">
         <v>142</v>
       </c>
       <c r="E480" s="35" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="F480" s="62" t="s">
         <v>180</v>
@@ -16106,19 +16114,19 @@
     </row>
     <row r="481" ht="14.25" customHeight="1">
       <c r="A481" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B481" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C481" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D481" s="33" t="s">
         <v>72</v>
       </c>
       <c r="E481" s="35" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F481" s="62" t="s">
         <v>180</v>
@@ -16132,19 +16140,19 @@
     </row>
     <row r="482" ht="14.25" customHeight="1">
       <c r="A482" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B482" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C482" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D482" s="33" t="s">
         <v>76</v>
       </c>
       <c r="E482" s="35" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="F482" s="62" t="s">
         <v>180</v>
@@ -16158,19 +16166,19 @@
     </row>
     <row r="483" ht="14.25" customHeight="1">
       <c r="A483" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B483" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C483" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D483" s="33" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="E483" s="35" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="F483" s="62" t="s">
         <v>180</v>
@@ -16184,19 +16192,19 @@
     </row>
     <row r="484" ht="14.25" customHeight="1">
       <c r="A484" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B484" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C484" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D484" s="33" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="E484" s="35" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F484" s="62" t="s">
         <v>180</v>
@@ -16210,19 +16218,19 @@
     </row>
     <row r="485" ht="14.25" customHeight="1">
       <c r="A485" s="44" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B485" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C485" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D485" s="49" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="E485" s="55" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="F485" s="62" t="s">
         <v>180</v>
@@ -16236,26 +16244,26 @@
     </row>
     <row r="486" ht="14.25" customHeight="1">
       <c r="A486" s="44" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B486" s="26" t="s">
         <v>87</v>
       </c>
       <c r="C486" s="52" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D486" s="49" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="E486" s="55" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="F486" s="15" t="s">
         <v>180</v>
       </c>
       <c r="G486" s="16"/>
       <c r="I486" s="76" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="J486" s="16"/>
       <c r="M486" s="8">
@@ -16267,25 +16275,27 @@
     </row>
     <row r="487" ht="14.25" customHeight="1">
       <c r="A487" s="44" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B487" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C487" s="61" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D487" s="33" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E487" s="35" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="F487" s="15" t="s">
         <v>90</v>
       </c>
       <c r="G487" s="16"/>
-      <c r="I487" s="21"/>
+      <c r="I487" s="41" t="s">
+        <v>808</v>
+      </c>
       <c r="J487" s="16"/>
       <c r="M487" s="8">
         <v>2.441056</v>
@@ -16296,19 +16306,19 @@
     </row>
     <row r="488" ht="14.25" customHeight="1">
       <c r="A488" s="44" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B488" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C488" s="61" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D488" s="33" t="s">
         <v>88</v>
       </c>
       <c r="E488" s="35" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="F488" s="15" t="s">
         <v>90</v>
@@ -16321,19 +16331,19 @@
     </row>
     <row r="489" ht="14.25" customHeight="1">
       <c r="A489" s="44" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B489" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C489" s="61" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D489" s="33" t="s">
         <v>22</v>
       </c>
       <c r="E489" s="35" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="F489" s="15" t="s">
         <v>90</v>
@@ -16346,19 +16356,19 @@
     </row>
     <row r="490" ht="14.25" customHeight="1">
       <c r="A490" s="44" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B490" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C490" s="61" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D490" s="33" t="s">
         <v>428</v>
       </c>
       <c r="E490" s="35" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="F490" s="15" t="s">
         <v>90</v>
@@ -16371,19 +16381,19 @@
     </row>
     <row r="491" ht="14.25" customHeight="1">
       <c r="A491" s="44" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B491" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C491" s="61" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D491" s="33" t="s">
         <v>240</v>
       </c>
       <c r="E491" s="35" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="F491" s="15" t="s">
         <v>90</v>
@@ -16396,19 +16406,19 @@
     </row>
     <row r="492" ht="14.25" customHeight="1">
       <c r="A492" s="44" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B492" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C492" s="61" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D492" s="33" t="s">
         <v>142</v>
       </c>
       <c r="E492" s="35" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="F492" s="15" t="s">
         <v>90</v>
@@ -16421,16 +16431,16 @@
     </row>
     <row r="493" ht="14.25" customHeight="1">
       <c r="A493" s="44" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B493" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C493" s="61" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D493" s="33" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="E493" s="77"/>
       <c r="F493" s="15" t="s">
@@ -16444,19 +16454,19 @@
     </row>
     <row r="494" ht="14.25" customHeight="1">
       <c r="A494" s="44" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B494" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C494" s="61" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D494" s="49" t="s">
         <v>72</v>
       </c>
       <c r="E494" s="55" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="F494" s="15" t="s">
         <v>90</v>
@@ -16469,26 +16479,26 @@
     </row>
     <row r="495" ht="15.75" customHeight="1">
       <c r="A495" s="44" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B495" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C495" s="78" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="D495" s="33" t="s">
         <v>136</v>
       </c>
       <c r="E495" s="35" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="F495" s="15" t="s">
         <v>180</v>
       </c>
       <c r="G495" s="16"/>
       <c r="I495" s="76" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="J495" s="16"/>
       <c r="M495" s="8">
@@ -16500,19 +16510,19 @@
     </row>
     <row r="496" ht="15.75" customHeight="1">
       <c r="A496" s="44" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B496" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C496" s="78" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="D496" s="33" t="s">
         <v>142</v>
       </c>
       <c r="E496" s="35" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="F496" s="15" t="s">
         <v>180</v>
@@ -16525,19 +16535,19 @@
     </row>
     <row r="497" ht="15.75" customHeight="1">
       <c r="A497" s="44" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B497" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C497" s="78" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="D497" s="33" t="s">
         <v>72</v>
       </c>
       <c r="E497" s="35" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="F497" s="15" t="s">
         <v>180</v>
@@ -16550,19 +16560,19 @@
     </row>
     <row r="498" ht="15.75" customHeight="1">
       <c r="A498" s="44" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B498" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C498" s="78" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="D498" s="33" t="s">
         <v>76</v>
       </c>
       <c r="E498" s="35" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="F498" s="15" t="s">
         <v>180</v>
@@ -16575,19 +16585,19 @@
     </row>
     <row r="499" ht="15.75" customHeight="1">
       <c r="A499" s="44" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B499" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C499" s="78" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="D499" s="33" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="E499" s="35" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="F499" s="15" t="s">
         <v>180</v>
@@ -16600,26 +16610,26 @@
     </row>
     <row r="500" ht="14.25" customHeight="1">
       <c r="A500" s="79" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="B500" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C500" s="80" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="D500" s="33" t="s">
         <v>17</v>
       </c>
       <c r="E500" s="14" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="F500" s="15" t="s">
         <v>90</v>
       </c>
       <c r="G500" s="16"/>
       <c r="I500" s="81" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="J500" s="16"/>
       <c r="M500" s="8">
@@ -16631,19 +16641,19 @@
     </row>
     <row r="501" ht="14.25" customHeight="1">
       <c r="A501" s="79" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="B501" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C501" s="80" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="D501" s="33" t="s">
         <v>531</v>
       </c>
       <c r="E501" s="14" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="F501" s="15" t="s">
         <v>90</v>
@@ -16656,19 +16666,19 @@
     </row>
     <row r="502" ht="14.25" customHeight="1">
       <c r="A502" s="79" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="B502" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C502" s="80" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="D502" s="33" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="E502" s="14" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="F502" s="15" t="s">
         <v>90</v>
@@ -16681,19 +16691,19 @@
     </row>
     <row r="503" ht="14.25" customHeight="1">
       <c r="A503" s="79" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="B503" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C503" s="80" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="D503" s="33" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="E503" s="14" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="F503" s="15" t="s">
         <v>90</v>
@@ -16706,19 +16716,19 @@
     </row>
     <row r="504" ht="14.25" customHeight="1">
       <c r="A504" s="79" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="B504" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C504" s="80" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="D504" s="33" t="s">
         <v>142</v>
       </c>
       <c r="E504" s="14" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="F504" s="15" t="s">
         <v>90</v>
@@ -16731,19 +16741,19 @@
     </row>
     <row r="505" ht="14.25" customHeight="1">
       <c r="A505" s="79" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="B505" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C505" s="80" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="D505" s="33" t="s">
         <v>72</v>
       </c>
       <c r="E505" s="14" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="F505" s="15" t="s">
         <v>90</v>
@@ -16756,19 +16766,19 @@
     </row>
     <row r="506" ht="14.25" customHeight="1">
       <c r="A506" s="79" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="B506" s="45" t="s">
         <v>526</v>
       </c>
       <c r="C506" s="80" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="D506" s="49" t="s">
         <v>428</v>
       </c>
       <c r="E506" s="14" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="F506" s="15" t="s">
         <v>90</v>
@@ -16781,29 +16791,29 @@
     </row>
     <row r="507" ht="14.25" customHeight="1">
       <c r="A507" s="82" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="B507" s="83" t="s">
         <v>526</v>
       </c>
       <c r="C507" s="84" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="D507" s="85" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="E507" s="86" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="F507" s="15" t="s">
         <v>180</v>
       </c>
       <c r="G507" s="16"/>
       <c r="H507" s="87" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="I507" s="88" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="J507" s="16"/>
       <c r="M507" s="8">
@@ -16815,29 +16825,29 @@
     </row>
     <row r="508" ht="14.25" customHeight="1">
       <c r="A508" s="89" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="B508" s="83" t="s">
         <v>526</v>
       </c>
       <c r="C508" s="90" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="D508" s="85" t="s">
         <v>72</v>
       </c>
       <c r="E508" s="86" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="F508" s="15" t="s">
         <v>180</v>
       </c>
       <c r="G508" s="16"/>
       <c r="H508" s="87" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="I508" s="91" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="J508" s="16"/>
       <c r="M508" s="8">
@@ -21708,70 +21718,71 @@
     <hyperlink r:id="rId458" ref="E451"/>
     <hyperlink r:id="rId459" ref="E452"/>
     <hyperlink r:id="rId460" ref="E453"/>
-    <hyperlink r:id="rId461" ref="E455"/>
-    <hyperlink r:id="rId462" ref="E456"/>
-    <hyperlink r:id="rId463" ref="E457"/>
-    <hyperlink r:id="rId464" ref="E458"/>
-    <hyperlink r:id="rId465" ref="E459"/>
-    <hyperlink r:id="rId466" ref="E460"/>
-    <hyperlink r:id="rId467" ref="E461"/>
-    <hyperlink r:id="rId468" ref="E462"/>
-    <hyperlink r:id="rId469" ref="E463"/>
-    <hyperlink r:id="rId470" ref="I463"/>
-    <hyperlink r:id="rId471" ref="E464"/>
-    <hyperlink r:id="rId472" ref="E465"/>
-    <hyperlink r:id="rId473" ref="E466"/>
-    <hyperlink r:id="rId474" ref="E467"/>
-    <hyperlink r:id="rId475" ref="E468"/>
-    <hyperlink r:id="rId476" ref="E469"/>
-    <hyperlink r:id="rId477" ref="E470"/>
-    <hyperlink r:id="rId478" ref="E471"/>
-    <hyperlink r:id="rId479" ref="E472"/>
-    <hyperlink r:id="rId480" ref="E473"/>
-    <hyperlink r:id="rId481" ref="E474"/>
-    <hyperlink r:id="rId482" ref="I474"/>
-    <hyperlink r:id="rId483" ref="E475"/>
-    <hyperlink r:id="rId484" ref="E476"/>
-    <hyperlink r:id="rId485" ref="E477"/>
-    <hyperlink r:id="rId486" ref="E478"/>
-    <hyperlink r:id="rId487" ref="E479"/>
-    <hyperlink r:id="rId488" ref="E480"/>
-    <hyperlink r:id="rId489" ref="E481"/>
-    <hyperlink r:id="rId490" ref="E482"/>
-    <hyperlink r:id="rId491" ref="E483"/>
-    <hyperlink r:id="rId492" ref="E484"/>
-    <hyperlink r:id="rId493" ref="E485"/>
-    <hyperlink r:id="rId494" ref="E486"/>
-    <hyperlink r:id="rId495" ref="I486"/>
-    <hyperlink r:id="rId496" ref="E487"/>
-    <hyperlink r:id="rId497" ref="E488"/>
-    <hyperlink r:id="rId498" ref="E489"/>
-    <hyperlink r:id="rId499" ref="E490"/>
-    <hyperlink r:id="rId500" ref="E491"/>
-    <hyperlink r:id="rId501" ref="E492"/>
-    <hyperlink r:id="rId502" ref="E494"/>
-    <hyperlink r:id="rId503" ref="E495"/>
-    <hyperlink r:id="rId504" ref="I495"/>
-    <hyperlink r:id="rId505" ref="E496"/>
-    <hyperlink r:id="rId506" ref="E497"/>
-    <hyperlink r:id="rId507" ref="E498"/>
-    <hyperlink r:id="rId508" ref="E499"/>
-    <hyperlink r:id="rId509" ref="E500"/>
-    <hyperlink r:id="rId510" ref="I500"/>
-    <hyperlink r:id="rId511" ref="E501"/>
-    <hyperlink r:id="rId512" ref="E502"/>
-    <hyperlink r:id="rId513" ref="E503"/>
-    <hyperlink r:id="rId514" ref="E504"/>
-    <hyperlink r:id="rId515" ref="E505"/>
-    <hyperlink r:id="rId516" ref="E506"/>
-    <hyperlink r:id="rId517" ref="E507"/>
-    <hyperlink r:id="rId518" ref="I507"/>
-    <hyperlink r:id="rId519" ref="E508"/>
+    <hyperlink r:id="rId461" ref="I454"/>
+    <hyperlink r:id="rId462" ref="E455"/>
+    <hyperlink r:id="rId463" ref="E456"/>
+    <hyperlink r:id="rId464" ref="E457"/>
+    <hyperlink r:id="rId465" ref="E458"/>
+    <hyperlink r:id="rId466" ref="E459"/>
+    <hyperlink r:id="rId467" ref="E460"/>
+    <hyperlink r:id="rId468" ref="E461"/>
+    <hyperlink r:id="rId469" ref="E462"/>
+    <hyperlink r:id="rId470" ref="E463"/>
+    <hyperlink r:id="rId471" ref="I463"/>
+    <hyperlink r:id="rId472" ref="E464"/>
+    <hyperlink r:id="rId473" ref="E465"/>
+    <hyperlink r:id="rId474" ref="E466"/>
+    <hyperlink r:id="rId475" ref="E467"/>
+    <hyperlink r:id="rId476" ref="E468"/>
+    <hyperlink r:id="rId477" ref="E469"/>
+    <hyperlink r:id="rId478" ref="E470"/>
+    <hyperlink r:id="rId479" ref="E471"/>
+    <hyperlink r:id="rId480" ref="E472"/>
+    <hyperlink r:id="rId481" ref="E473"/>
+    <hyperlink r:id="rId482" ref="E474"/>
+    <hyperlink r:id="rId483" ref="I474"/>
+    <hyperlink r:id="rId484" ref="E475"/>
+    <hyperlink r:id="rId485" ref="E476"/>
+    <hyperlink r:id="rId486" ref="E477"/>
+    <hyperlink r:id="rId487" ref="E478"/>
+    <hyperlink r:id="rId488" ref="E479"/>
+    <hyperlink r:id="rId489" ref="E480"/>
+    <hyperlink r:id="rId490" ref="E481"/>
+    <hyperlink r:id="rId491" ref="E482"/>
+    <hyperlink r:id="rId492" ref="E483"/>
+    <hyperlink r:id="rId493" ref="E484"/>
+    <hyperlink r:id="rId494" ref="E485"/>
+    <hyperlink r:id="rId495" ref="E486"/>
+    <hyperlink r:id="rId496" ref="I486"/>
+    <hyperlink r:id="rId497" ref="E487"/>
+    <hyperlink r:id="rId498" ref="E488"/>
+    <hyperlink r:id="rId499" ref="E489"/>
+    <hyperlink r:id="rId500" ref="E490"/>
+    <hyperlink r:id="rId501" ref="E491"/>
+    <hyperlink r:id="rId502" ref="E492"/>
+    <hyperlink r:id="rId503" ref="E494"/>
+    <hyperlink r:id="rId504" ref="E495"/>
+    <hyperlink r:id="rId505" ref="I495"/>
+    <hyperlink r:id="rId506" ref="E496"/>
+    <hyperlink r:id="rId507" ref="E497"/>
+    <hyperlink r:id="rId508" ref="E498"/>
+    <hyperlink r:id="rId509" ref="E499"/>
+    <hyperlink r:id="rId510" ref="E500"/>
+    <hyperlink r:id="rId511" ref="I500"/>
+    <hyperlink r:id="rId512" ref="E501"/>
+    <hyperlink r:id="rId513" ref="E502"/>
+    <hyperlink r:id="rId514" ref="E503"/>
+    <hyperlink r:id="rId515" ref="E504"/>
+    <hyperlink r:id="rId516" ref="E505"/>
+    <hyperlink r:id="rId517" ref="E506"/>
+    <hyperlink r:id="rId518" ref="E507"/>
+    <hyperlink r:id="rId519" ref="I507"/>
+    <hyperlink r:id="rId520" ref="E508"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId520"/>
-  <legacyDrawing r:id="rId521"/>
+  <drawing r:id="rId521"/>
+  <legacyDrawing r:id="rId522"/>
 </worksheet>
 </file>
</xml_diff>